<commit_message>
update upload stocker manual format and delete stocker id tools
</commit_message>
<xml_diff>
--- a/public/assets/example/contoh-import-stocker-manual.xlsx
+++ b/public/assets/example/contoh-import-stocker-manual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7620"/>
+    <workbookView windowWidth="19545" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>act_costing_ws</t>
   </si>
@@ -44,6 +44,9 @@
     <t>part_detail</t>
   </si>
   <si>
+    <t>proses</t>
+  </si>
+  <si>
     <t>shade</t>
   </si>
   <si>
@@ -77,16 +80,22 @@
     <t>no_bon_loading</t>
   </si>
   <si>
-    <t>PTX/1023/086</t>
-  </si>
-  <si>
-    <t>BLACK</t>
-  </si>
-  <si>
-    <t>FRONT BODY</t>
-  </si>
-  <si>
-    <t>PANTS</t>
+    <t>CON/0825/022</t>
+  </si>
+  <si>
+    <t>K0111506 EVERBLUE</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>BODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BODY - TOP	</t>
+  </si>
+  <si>
+    <t>TROLLEY</t>
   </si>
   <si>
     <t>-</t>
@@ -96,6 +105,60 @@
   </si>
   <si>
     <t>line</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>87395</t>
+  </si>
+  <si>
+    <t>CON/0825/027</t>
+  </si>
+  <si>
+    <t>K0122605 WHITE/ATLANTA BLUE</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>MAIN BODY</t>
+  </si>
+  <si>
+    <t>BLK PRINT - TOP</t>
+  </si>
+  <si>
+    <t>PRINT</t>
+  </si>
+  <si>
+    <t>87398</t>
+  </si>
+  <si>
+    <t>CON/0825/025</t>
+  </si>
+  <si>
+    <t>K0122502 ATLANTA BLUE/WHITE</t>
+  </si>
+  <si>
+    <t>87397</t>
+  </si>
+  <si>
+    <t>CON/0825/015</t>
+  </si>
+  <si>
+    <t>K0123404 VAPOR BLUE</t>
+  </si>
+  <si>
+    <t>BLK HEATSEAL - TOP</t>
+  </si>
+  <si>
+    <t>HEATSEAL</t>
+  </si>
+  <si>
+    <t>92004</t>
+  </si>
+  <si>
+    <t>K0123401 WHITE</t>
   </si>
 </sst>
 </file>
@@ -108,7 +171,12 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -569,154 +637,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,577 +1325,346 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="15.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="9.85714285714286" customWidth="1"/>
-    <col min="7" max="7" width="10.4285714285714" customWidth="1"/>
-    <col min="8" max="8" width="18.7142857142857" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="18.5714285714286" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="17.7142857142857" customWidth="1"/>
-    <col min="14" max="14" width="20.1428571428571" customWidth="1"/>
-    <col min="15" max="15" width="12.8571428571429" customWidth="1"/>
-    <col min="16" max="16" width="16.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="16.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42857142857143" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.2857142857143" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28571428571429" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28571428571429" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85714285714286" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7142857142857" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1428571428571" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.4285714285714" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:17">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2">
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>45919</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>27</v>
-      </c>
-      <c r="K2">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>29</v>
-      </c>
-      <c r="M2">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O2">
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3</v>
+      </c>
+      <c r="N3" s="3">
+        <v>3</v>
+      </c>
+      <c r="O3" s="4">
+        <v>45919</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>1234</v>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>45919</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
+    <row r="5" spans="1:17">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>27</v>
-      </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-      <c r="L3">
-        <v>29</v>
-      </c>
-      <c r="M3">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1234</v>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4">
+        <v>45919</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4">
+    <row r="6" spans="1:17">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4">
-        <v>27</v>
-      </c>
-      <c r="K4">
-        <v>28</v>
-      </c>
-      <c r="L4">
-        <v>29</v>
-      </c>
-      <c r="M4">
-        <v>29</v>
-      </c>
-      <c r="N4" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5">
-        <v>27</v>
-      </c>
-      <c r="K5">
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <v>29</v>
-      </c>
-      <c r="M5">
-        <v>29</v>
-      </c>
-      <c r="N5" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6">
-        <v>27</v>
-      </c>
-      <c r="K6">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>29</v>
-      </c>
-      <c r="M6">
-        <v>29</v>
-      </c>
-      <c r="N6" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7">
-        <v>27</v>
-      </c>
-      <c r="K7">
-        <v>28</v>
-      </c>
-      <c r="L7">
-        <v>29</v>
-      </c>
-      <c r="M7">
-        <v>29</v>
-      </c>
-      <c r="N7" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8">
-        <v>27</v>
-      </c>
-      <c r="K8">
-        <v>28</v>
-      </c>
-      <c r="L8">
-        <v>29</v>
-      </c>
-      <c r="M8">
-        <v>29</v>
-      </c>
-      <c r="N8" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9">
-        <v>27</v>
-      </c>
-      <c r="K9">
-        <v>28</v>
-      </c>
-      <c r="L9">
-        <v>29</v>
-      </c>
-      <c r="M9">
-        <v>29</v>
-      </c>
-      <c r="N9" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10">
-        <v>27</v>
-      </c>
-      <c r="K10">
-        <v>28</v>
-      </c>
-      <c r="L10">
-        <v>29</v>
-      </c>
-      <c r="M10">
-        <v>29</v>
-      </c>
-      <c r="N10" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11">
-        <v>27</v>
-      </c>
-      <c r="K11">
-        <v>28</v>
-      </c>
-      <c r="L11">
-        <v>29</v>
-      </c>
-      <c r="M11">
-        <v>29</v>
-      </c>
-      <c r="N11" s="1">
-        <v>45875</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>1234</v>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" s="3">
+        <v>4</v>
+      </c>
+      <c r="O6" s="4">
+        <v>45919</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>